<commit_message>
Updated for shortened Summer 2 session
</commit_message>
<xml_diff>
--- a/MSDS_Courses.xlsx
+++ b/MSDS_Courses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e79b3e2af0eb62e/Documents/GitHub/MSDS_Coursework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1385" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBF12B84-55F5-462B-A045-BC332DFC0B05}"/>
+  <xr:revisionPtr revIDLastSave="1513" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9E0CB65-634D-44D2-8BDD-F1AAC2895D2C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="179">
   <si>
     <t>Specialization</t>
   </si>
@@ -542,28 +542,43 @@
     <t>Successful Presentation</t>
   </si>
   <si>
-    <t>2025 Spring 1</t>
-  </si>
-  <si>
-    <t>2025 Spring 2</t>
-  </si>
-  <si>
-    <t>2025 Summer 1</t>
-  </si>
-  <si>
-    <t>2025 Summer 2</t>
-  </si>
-  <si>
-    <t>2025 Fall 1</t>
-  </si>
-  <si>
-    <t>2025 Fall 2</t>
-  </si>
-  <si>
     <t>2026 Spring 1</t>
   </si>
   <si>
     <t>2026 Spring 2</t>
+  </si>
+  <si>
+    <t>Natural Language Processing</t>
+  </si>
+  <si>
+    <t>Statistical Modeling</t>
+  </si>
+  <si>
+    <t>Statistical Learning</t>
+  </si>
+  <si>
+    <t>2025 Summer 2 (5 weeks)</t>
+  </si>
+  <si>
+    <t>Summer Break (Pay Coursera) (3 weeks)</t>
+  </si>
+  <si>
+    <t>2025 Fall 2 (8 weeks)</t>
+  </si>
+  <si>
+    <t>2025 Fall 1 (7 weeks)</t>
+  </si>
+  <si>
+    <t>2025 Summer 1 (7 weeks)</t>
+  </si>
+  <si>
+    <t>2025 Spring 2 (8 weeks)</t>
+  </si>
+  <si>
+    <t>2025 Spring 1 (7 weeks)</t>
+  </si>
+  <si>
+    <t>* Apply for jobs</t>
   </si>
 </sst>
 </file>
@@ -593,7 +608,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -603,6 +618,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -619,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -634,26 +709,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCFF"/>
+      <color rgb="FFCCCCFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -936,18 +1018,18 @@
   <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A48" sqref="A48:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.21875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="8"/>
-    <col min="6" max="6" width="10.44140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" style="1" customWidth="1"/>
@@ -963,19 +1045,19 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="10" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="3" t="s">
         <v>161</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -1010,19 +1092,19 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8">
-        <v>1</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="8">
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1">
         <v>20</v>
       </c>
       <c r="G2" s="1">
@@ -1057,19 +1139,19 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
         <v>25</v>
       </c>
       <c r="G3" s="1">
@@ -1104,19 +1186,19 @@
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1">
         <v>16</v>
       </c>
       <c r="G4" s="1">
@@ -1147,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -1194,23 +1276,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="8">
-        <v>1</v>
-      </c>
-      <c r="C6" s="7" t="s">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1">
         <v>17</v>
       </c>
       <c r="G6" s="1">
@@ -1241,23 +1323,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="1">
         <v>2</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1">
         <v>9</v>
       </c>
       <c r="G7" s="1">
@@ -1288,23 +1370,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="1">
         <v>3</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1">
         <v>16</v>
       </c>
       <c r="G8" s="1">
@@ -1335,23 +1417,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="1">
         <v>4</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" t="s">
         <v>80</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1">
         <v>48</v>
       </c>
       <c r="G9" s="1">
@@ -1382,23 +1464,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="1">
         <v>5</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" t="s">
         <v>82</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1">
         <v>44</v>
       </c>
       <c r="G10" s="1">
@@ -1429,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>48</v>
       </c>
@@ -1476,23 +1558,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="1">
         <v>3</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1">
         <v>16</v>
       </c>
       <c r="G12" s="1">
@@ -1523,23 +1605,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>60</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" t="s">
         <v>163</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="8">
+      <c r="E13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="1">
         <v>12</v>
       </c>
       <c r="G13" s="1">
@@ -1570,23 +1652,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="1">
         <v>2</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" t="s">
         <v>164</v>
       </c>
-      <c r="E14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="8">
+      <c r="E14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="1">
         <v>29</v>
       </c>
       <c r="G14" s="1">
@@ -1617,23 +1699,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>59</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="1">
         <v>3</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" t="s">
         <v>162</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" t="s">
         <v>165</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="8">
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1">
         <v>20</v>
       </c>
       <c r="G15" s="1">
@@ -1664,23 +1746,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="1">
         <v>4</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1">
         <v>13</v>
       </c>
       <c r="G16" s="1">
@@ -1711,23 +1793,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="8">
-        <v>1</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1">
         <v>20</v>
       </c>
       <c r="G17" s="1">
@@ -1758,23 +1840,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1">
         <v>17</v>
       </c>
       <c r="G18" s="1">
@@ -1805,23 +1887,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="1">
         <v>3</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="8">
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="1">
         <v>13</v>
       </c>
       <c r="G19" s="1">
@@ -1852,23 +1934,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="8">
-        <v>1</v>
-      </c>
-      <c r="C20" s="7" t="s">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" t="s">
         <v>72</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="8">
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1">
         <v>8</v>
       </c>
       <c r="G20" s="1">
@@ -1899,23 +1981,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="8">
+      <c r="B21" s="1">
         <v>2</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="1">
         <v>10</v>
       </c>
       <c r="G21" s="1">
@@ -1946,23 +2028,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B22" s="1">
         <v>3</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="8">
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1">
         <v>10</v>
       </c>
       <c r="G22" s="1">
@@ -1997,19 +2079,19 @@
       <c r="A23" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="8">
-        <v>1</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F23" s="8">
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="1">
         <v>27</v>
       </c>
       <c r="G23" s="1">
@@ -2044,19 +2126,19 @@
       <c r="A24" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" t="s">
         <v>94</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" t="s">
         <v>95</v>
       </c>
-      <c r="E24" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="8">
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="1">
         <v>25</v>
       </c>
       <c r="G24" s="1">
@@ -2091,19 +2173,19 @@
       <c r="A25" t="s">
         <v>91</v>
       </c>
-      <c r="B25" s="8">
+      <c r="B25" s="1">
         <v>3</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" t="s">
         <v>96</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" t="s">
         <v>97</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="8">
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1">
         <v>42</v>
       </c>
       <c r="G25" s="1">
@@ -2134,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>98</v>
       </c>
@@ -2181,7 +2263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>98</v>
       </c>
@@ -2228,7 +2310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>98</v>
       </c>
@@ -2275,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>105</v>
       </c>
@@ -2322,7 +2404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>105</v>
       </c>
@@ -2369,7 +2451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>105</v>
       </c>
@@ -2416,23 +2498,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="8">
-        <v>1</v>
-      </c>
-      <c r="C32" s="7" t="s">
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" t="s">
         <v>114</v>
       </c>
-      <c r="E32" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="8">
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1">
         <v>19</v>
       </c>
       <c r="G32" s="1">
@@ -2463,23 +2545,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
+    <row r="33" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="8">
+      <c r="B33" s="1">
         <v>2</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" t="s">
         <v>115</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" t="s">
         <v>116</v>
       </c>
-      <c r="E33" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="8">
+      <c r="E33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="1">
         <v>17</v>
       </c>
       <c r="G33" s="1">
@@ -2510,7 +2592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>117</v>
       </c>
@@ -2557,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>117</v>
       </c>
@@ -2604,23 +2686,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>124</v>
       </c>
-      <c r="B36" s="8">
-        <v>1</v>
-      </c>
-      <c r="C36" s="7" t="s">
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" t="s">
         <v>126</v>
       </c>
-      <c r="E36" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="8">
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="1">
         <v>23</v>
       </c>
       <c r="G36" s="1">
@@ -2651,23 +2733,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+    <row r="37" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>124</v>
       </c>
-      <c r="B37" s="8">
+      <c r="B37" s="1">
         <v>2</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" t="s">
         <v>127</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" t="s">
         <v>128</v>
       </c>
-      <c r="E37" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="8">
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="1">
         <v>26</v>
       </c>
       <c r="G37" s="1">
@@ -2698,23 +2780,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" s="7" t="s">
+    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>124</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="1">
         <v>3</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" t="s">
         <v>129</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" t="s">
         <v>130</v>
       </c>
-      <c r="E38" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="8">
+      <c r="E38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="1">
         <v>18</v>
       </c>
       <c r="G38" s="1">
@@ -2749,19 +2831,19 @@
       <c r="A39" t="s">
         <v>57</v>
       </c>
-      <c r="B39" s="8">
-        <v>1</v>
-      </c>
-      <c r="C39" s="7" t="s">
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
         <v>85</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" t="s">
         <v>86</v>
       </c>
-      <c r="E39" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="8">
+      <c r="E39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="1">
         <v>11</v>
       </c>
       <c r="G39" s="1">
@@ -2796,19 +2878,19 @@
       <c r="A40" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="8">
-        <v>1</v>
-      </c>
-      <c r="C40" s="7" t="s">
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" t="s">
         <v>88</v>
       </c>
-      <c r="E40" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" s="8">
+      <c r="E40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" s="1">
         <v>10</v>
       </c>
       <c r="G40" s="1">
@@ -2839,7 +2921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>57</v>
       </c>
@@ -2886,23 +2968,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="8">
-        <v>1</v>
-      </c>
-      <c r="C42" s="7" t="s">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
         <v>89</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" t="s">
         <v>90</v>
       </c>
-      <c r="E42" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="8">
+      <c r="E42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="1">
         <v>18</v>
       </c>
       <c r="G42" s="1">
@@ -2933,23 +3015,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="8">
-        <v>1</v>
-      </c>
-      <c r="C43" s="7" t="s">
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" t="s">
         <v>55</v>
       </c>
-      <c r="E43" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="8">
+      <c r="E43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="1">
         <v>20</v>
       </c>
       <c r="G43" s="1">
@@ -2984,19 +3066,19 @@
       <c r="A44" t="s">
         <v>57</v>
       </c>
-      <c r="B44" s="8">
-        <v>1</v>
-      </c>
-      <c r="C44" s="7" t="s">
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
         <v>122</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" t="s">
         <v>123</v>
       </c>
-      <c r="E44" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="8">
+      <c r="E44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="1">
         <v>18</v>
       </c>
       <c r="G44" s="1">
@@ -3027,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>30</v>
       </c>
@@ -3074,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>30</v>
       </c>
@@ -3121,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>30</v>
       </c>
@@ -3168,7 +3250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>131</v>
       </c>
@@ -3215,23 +3297,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" s="7" t="s">
+    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>131</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="1">
         <v>2</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" t="s">
         <v>134</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" t="s">
         <v>135</v>
       </c>
-      <c r="E49" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="8">
+      <c r="E49" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="1">
         <v>15</v>
       </c>
       <c r="G49" s="1">
@@ -3262,23 +3344,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
+    <row r="50" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>131</v>
       </c>
-      <c r="B50" s="8">
+      <c r="B50" s="1">
         <v>3</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" t="s">
         <v>136</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" t="s">
         <v>137</v>
       </c>
-      <c r="E50" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="8">
+      <c r="E50" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" s="1">
         <v>12</v>
       </c>
       <c r="G50" s="1">
@@ -3309,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>138</v>
       </c>
@@ -3356,7 +3438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>138</v>
       </c>
@@ -3403,23 +3485,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="7" t="s">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>138</v>
       </c>
-      <c r="B53" s="8">
+      <c r="B53" s="1">
         <v>3</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" t="s">
         <v>143</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" t="s">
         <v>144</v>
       </c>
-      <c r="E53" s="8" t="s">
+      <c r="E53" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F53" s="1">
         <v>42</v>
       </c>
       <c r="G53" s="1">
@@ -3450,23 +3532,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>145</v>
       </c>
-      <c r="B54" s="8">
-        <v>1</v>
-      </c>
-      <c r="C54" s="7" t="s">
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
         <v>146</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" t="s">
         <v>147</v>
       </c>
-      <c r="E54" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F54" s="8">
+      <c r="E54" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="1">
         <v>12</v>
       </c>
       <c r="G54" s="1">
@@ -3497,23 +3579,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>145</v>
       </c>
-      <c r="B55" s="8">
+      <c r="B55" s="1">
         <v>2</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" t="s">
         <v>148</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" t="s">
         <v>149</v>
       </c>
-      <c r="E55" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F55" s="8">
+      <c r="E55" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="1">
         <v>13</v>
       </c>
       <c r="G55" s="1">
@@ -3544,23 +3626,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>145</v>
       </c>
-      <c r="B56" s="8">
+      <c r="B56" s="1">
         <v>3</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" t="s">
         <v>150</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" t="s">
         <v>151</v>
       </c>
-      <c r="E56" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F56" s="8">
+      <c r="E56" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="1">
         <v>10</v>
       </c>
       <c r="G56" s="1">
@@ -3591,7 +3673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>152</v>
       </c>
@@ -3638,7 +3720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>152</v>
       </c>
@@ -3689,7 +3771,7 @@
   <autoFilter ref="A1:O58" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="4">
       <filters>
-        <filter val="Elective"/>
+        <filter val="Core"/>
       </filters>
     </filterColumn>
     <filterColumn colId="12">
@@ -3829,22 +3911,22 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="1">
         <v>24</v>
       </c>
       <c r="G3" s="1">
@@ -4111,22 +4193,22 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" t="s">
         <v>152</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" t="s">
         <v>155</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="1">
         <v>19</v>
       </c>
       <c r="G9" s="1">
@@ -4172,10 +4254,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D5ACC4-4F75-46C3-931B-94A525DB3F50}">
-  <dimension ref="A1:G49"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4186,6 +4268,7 @@
     <col min="4" max="4" width="39.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
     <col min="6" max="6" width="9.88671875" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
@@ -4208,24 +4291,25 @@
         <v>161</v>
       </c>
       <c r="G1">
-        <f>SUM(G2:G60)</f>
+        <f>SUM(G2:G61)</f>
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="9">
-        <v>210</v>
+      <c r="A2" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="6">
+        <f>SUM(F3:F5)</f>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="1">
@@ -4248,7 +4332,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B4" s="1">
@@ -4271,7 +4355,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B5" s="1">
@@ -4294,19 +4378,20 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="9">
-        <v>222</v>
+      <c r="A6" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="6">
+        <f>SUM(F7:F11)</f>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="1">
@@ -4329,7 +4414,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1">
@@ -4352,7 +4437,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B9" s="1">
@@ -4375,7 +4460,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="8" t="s">
         <v>152</v>
       </c>
       <c r="B10" s="1">
@@ -4398,7 +4483,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="8" t="s">
         <v>152</v>
       </c>
       <c r="B11" s="1">
@@ -4421,19 +4506,20 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="9">
-        <v>204</v>
+      <c r="A12" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="6">
+        <f>SUM(F13:F16)</f>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B13" s="1">
@@ -4456,7 +4542,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="8" t="s">
         <v>152</v>
       </c>
       <c r="B14" s="1">
@@ -4479,7 +4565,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" s="8" t="s">
         <v>152</v>
       </c>
       <c r="B15" s="1">
@@ -4502,7 +4588,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="10" t="s">
         <v>48</v>
       </c>
       <c r="B16" s="1">
@@ -4524,20 +4610,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="9">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="6">
+        <f>SUM(F18:F23)</f>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="1">
@@ -4558,274 +4645,298 @@
       <c r="G18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="H18" t="s">
         <v>30</v>
+      </c>
+      <c r="I18">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="1">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>13</v>
+      <c r="H19" t="s">
+        <v>168</v>
+      </c>
+      <c r="I19">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>105</v>
       </c>
       <c r="B20" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>21</v>
+        <v>106</v>
       </c>
       <c r="D20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1">
+        <v>14</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="1">
+        <v>7</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1">
         <v>22</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="1">
-        <v>19</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" t="s">
-        <v>84</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="1">
-        <v>8</v>
-      </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>105</v>
-      </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" t="s">
-        <v>107</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="1">
-        <v>14</v>
-      </c>
       <c r="G22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>105</v>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>117</v>
       </c>
       <c r="B23" s="1">
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="D23" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="1">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G23">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="6">
+        <f>SUM(F25:F27)</f>
+        <v>67</v>
+      </c>
+      <c r="H24" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="1">
+        <v>36</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B26" s="1">
         <v>3</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>110</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D26" t="s">
         <v>111</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="1">
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="1">
         <v>23</v>
       </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="1">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>118</v>
-      </c>
-      <c r="D25" t="s">
-        <v>119</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="1">
-        <v>22</v>
-      </c>
-      <c r="G25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>117</v>
-      </c>
-      <c r="B26" s="1">
-        <v>2</v>
-      </c>
-      <c r="C26" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" t="s">
-        <v>121</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="1">
-        <v>19</v>
-      </c>
       <c r="G26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="9">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="1">
+        <v>8</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="6">
+        <f>SUM(F29:F32)</f>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="1">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
         <v>99</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>100</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="1">
-        <v>39</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>98</v>
-      </c>
-      <c r="B29" s="1">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>101</v>
-      </c>
-      <c r="D29" t="s">
-        <v>102</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F29" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="G29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="H29" t="s">
         <v>98</v>
       </c>
+      <c r="I29">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="13" t="s">
+        <v>98</v>
+      </c>
       <c r="B30" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D30" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F30" s="1">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="G30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="H30" t="s">
+        <v>169</v>
+      </c>
+      <c r="I30">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
         <v>138</v>
       </c>
       <c r="B31" s="1">
@@ -4846,172 +4957,221 @@
       <c r="G31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="9">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="H31" t="s">
+        <v>170</v>
+      </c>
+      <c r="I31">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" t="s">
+        <v>133</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1">
+        <v>34</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="6">
+        <f>SUM(F34:F38)</f>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B34" s="1">
         <v>2</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>141</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>142</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="1">
-        <v>39</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>138</v>
-      </c>
-      <c r="B34" s="1">
-        <v>3</v>
-      </c>
-      <c r="C34" t="s">
-        <v>143</v>
-      </c>
-      <c r="D34" t="s">
-        <v>144</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F34" s="1">
+        <v>39</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>98</v>
+      </c>
+      <c r="I34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="1">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" t="s">
+        <v>144</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="1">
         <v>42</v>
       </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>169</v>
+      </c>
+      <c r="I35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="1">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="1">
+        <v>60</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>170</v>
+      </c>
+      <c r="I36">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B35" s="1">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>132</v>
-      </c>
-      <c r="D35" t="s">
-        <v>133</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" s="1">
-        <v>34</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="B37" s="1">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>134</v>
+      </c>
+      <c r="D37" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="1">
+        <v>15</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B36" s="1">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>134</v>
-      </c>
-      <c r="D36" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="1">
-        <v>15</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>131</v>
-      </c>
-      <c r="B37" s="1">
+      <c r="B38" s="1">
         <v>3</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>136</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>137</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="1">
+      <c r="E38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="1">
         <v>12</v>
       </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="9">
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="6">
         <v>240</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="6">
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.3">
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Summer 2 courses completed
</commit_message>
<xml_diff>
--- a/MSDS_Courses.xlsx
+++ b/MSDS_Courses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e79b3e2af0eb62e/Documents/GitHub/MSDS_Coursework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1769" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA237A0D-578F-4072-A73F-9B46671C3A80}"/>
+  <xr:revisionPtr revIDLastSave="1785" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61239C8F-F6F7-4DBA-A4BF-0EBBCC93064F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="174">
   <si>
     <t>Specialization</t>
   </si>
@@ -703,18 +703,18 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,10 +736,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1005,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDCB567-5E07-42C0-8D3A-079FDCB96AF6}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,19 +1071,19 @@
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="17">
-        <v>1</v>
-      </c>
-      <c r="C2" s="18" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="1">
         <v>40</v>
       </c>
       <c r="G2" s="1">
@@ -1119,115 +1115,112 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="20">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="20">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>152</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>153</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D5" t="s">
         <v>154</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F5" s="1">
         <v>10</v>
       </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1">
-        <v>0</v>
-      </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-      <c r="M3" s="1">
-        <v>0</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>155</v>
-      </c>
-      <c r="D4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-      <c r="M4" s="1">
-        <v>0</v>
-      </c>
-      <c r="N4" s="1">
-        <v>1</v>
-      </c>
-      <c r="O4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B5" s="17">
-        <v>3</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="17">
-        <v>23</v>
-      </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
@@ -1253,30 +1246,30 @@
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>152</v>
       </c>
       <c r="B6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>155</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>156</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F6" s="1">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -1300,30 +1293,27 @@
         <v>1</v>
       </c>
       <c r="O6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>20</v>
-      </c>
       <c r="B7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>157</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>158</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F7" s="1">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
@@ -1344,80 +1334,77 @@
         <v>0</v>
       </c>
       <c r="N7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O7" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="B8" s="20">
+        <v>4</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="1">
-        <v>37</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="1">
-        <v>0</v>
-      </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
-        <v>0</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0</v>
-      </c>
-      <c r="M8" s="1">
-        <v>0</v>
-      </c>
-      <c r="N8" s="1">
-        <v>1</v>
-      </c>
-      <c r="O8" s="1">
-        <v>0</v>
+      <c r="F8" s="20">
+        <v>14</v>
+      </c>
+      <c r="G8" s="20">
+        <v>0</v>
+      </c>
+      <c r="H8" s="20">
+        <v>0</v>
+      </c>
+      <c r="I8" s="20">
+        <v>0</v>
+      </c>
+      <c r="J8" s="20">
+        <v>0</v>
+      </c>
+      <c r="K8" s="20">
+        <v>0</v>
+      </c>
+      <c r="L8" s="20">
+        <v>0</v>
+      </c>
+      <c r="M8" s="20">
+        <v>0</v>
+      </c>
+      <c r="N8" s="20">
+        <v>1</v>
+      </c>
+      <c r="O8" s="20">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="1">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="G9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="1">
         <v>0</v>
@@ -1429,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1">
         <v>0</v>
@@ -1446,25 +1433,25 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="1">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="G10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
@@ -1476,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="1">
         <v>0</v>
@@ -1488,27 +1475,30 @@
         <v>1</v>
       </c>
       <c r="O10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="17">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1">
         <v>3</v>
       </c>
-      <c r="C11" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="17" t="s">
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="17">
-        <v>19</v>
+      <c r="F11" s="1">
+        <v>37</v>
       </c>
       <c r="G11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
@@ -1537,227 +1527,456 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F12" s="1">
+        <v>21</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1">
+        <v>24</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0</v>
+      </c>
+      <c r="N13" s="1">
+        <v>1</v>
+      </c>
+      <c r="O13" s="1">
+        <v>1</v>
+      </c>
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="1">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="1">
+        <v>19</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0</v>
+      </c>
+      <c r="L14" s="1">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1</v>
+      </c>
+      <c r="O14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="20">
+        <v>1</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="20">
+        <v>17</v>
+      </c>
+      <c r="G15" s="20">
+        <v>1</v>
+      </c>
+      <c r="H15" s="20">
+        <v>1</v>
+      </c>
+      <c r="I15" s="20">
+        <v>1</v>
+      </c>
+      <c r="J15" s="20">
+        <v>1</v>
+      </c>
+      <c r="K15" s="20">
+        <v>0</v>
+      </c>
+      <c r="L15" s="20">
+        <v>0</v>
+      </c>
+      <c r="M15" s="20">
+        <v>0</v>
+      </c>
+      <c r="N15" s="20">
+        <v>0</v>
+      </c>
+      <c r="O15" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="20">
+        <v>2</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="20">
+        <v>9</v>
+      </c>
+      <c r="G16" s="20">
+        <v>1</v>
+      </c>
+      <c r="H16" s="20">
+        <v>1</v>
+      </c>
+      <c r="I16" s="20">
+        <v>1</v>
+      </c>
+      <c r="J16" s="20">
+        <v>1</v>
+      </c>
+      <c r="K16" s="20">
+        <v>0</v>
+      </c>
+      <c r="L16" s="20">
+        <v>0</v>
+      </c>
+      <c r="M16" s="20">
+        <v>0</v>
+      </c>
+      <c r="N16" s="20">
+        <v>0</v>
+      </c>
+      <c r="O16" s="20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="1">
         <v>34</v>
       </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>0</v>
-      </c>
-      <c r="L12" s="1">
-        <v>0</v>
-      </c>
-      <c r="M12" s="1">
-        <v>0</v>
-      </c>
-      <c r="N12" s="1">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="17">
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
+        <v>0</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="O17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D18" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E18" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F18" s="1">
         <v>27</v>
       </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0</v>
-      </c>
-      <c r="I13" s="1">
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="1">
-        <v>0</v>
-      </c>
-      <c r="M13" s="1">
-        <v>0</v>
-      </c>
-      <c r="N13" s="1">
-        <v>0</v>
-      </c>
-      <c r="O13" s="1">
-        <v>0</v>
-      </c>
-      <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="17">
-        <v>1</v>
-      </c>
-      <c r="C14" s="18" t="s">
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D19" t="s">
         <v>107</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="17">
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="1">
         <v>14</v>
       </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>0</v>
-      </c>
-      <c r="K14" s="1">
-        <v>0</v>
-      </c>
-      <c r="L14" s="1">
-        <v>0</v>
-      </c>
-      <c r="M14" s="1">
-        <v>0</v>
-      </c>
-      <c r="N14" s="1">
-        <v>0</v>
-      </c>
-      <c r="O14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="17">
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0</v>
+      </c>
+      <c r="P19" s="19"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C20" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D20" t="s">
         <v>109</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="17">
-        <v>7</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0</v>
-      </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
-      <c r="K15" s="1">
-        <v>0</v>
-      </c>
-      <c r="L15" s="1">
-        <v>0</v>
-      </c>
-      <c r="M15" s="1">
-        <v>0</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0</v>
-      </c>
-      <c r="O15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="17">
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1">
+        <v>7</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1">
+        <v>0</v>
+      </c>
+      <c r="P20" s="19"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B21" s="1">
         <v>3</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C21" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D21" t="s">
         <v>111</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="17">
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" s="1">
         <v>23</v>
       </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-      <c r="I16" s="1">
-        <v>0</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
-        <v>0</v>
-      </c>
-      <c r="L16" s="1">
-        <v>0</v>
-      </c>
-      <c r="M16" s="1">
-        <v>0</v>
-      </c>
-      <c r="N16" s="1">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1">
-        <v>0</v>
-      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+      <c r="P21" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O16" xr:uid="{6FDCB567-5E07-42C0-8D3A-079FDCB96AF6}">
@@ -1765,8 +1984,8 @@
       <sortCondition ref="C1:C9"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O9">
-    <sortCondition ref="A1:A9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O21">
+    <sortCondition ref="C1:C21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1774,11 +1993,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:F20"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1988,22 +2207,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="20">
+        <v>1</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="5">
+      <c r="E5" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="20">
         <v>17</v>
       </c>
       <c r="G5" s="1">
@@ -2035,22 +2254,22 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="20">
         <v>2</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="5">
+      <c r="E6" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="20">
         <v>9</v>
       </c>
       <c r="G6" s="1">
@@ -2458,22 +2677,22 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="18" t="s">
+      <c r="A15" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="17">
-        <v>1</v>
-      </c>
-      <c r="C15" s="18" t="s">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="17">
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1">
         <v>20</v>
       </c>
       <c r="G15" s="1">
@@ -2505,22 +2724,22 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="18" t="s">
+      <c r="A16" t="s">
         <v>63</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="17">
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1">
         <v>17</v>
       </c>
       <c r="G16" s="1">
@@ -2552,22 +2771,22 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
+      <c r="A17" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="1">
         <v>3</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="17">
+      <c r="E17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="1">
         <v>13</v>
       </c>
       <c r="G17" s="1">
@@ -3116,22 +3335,22 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="18" t="s">
+      <c r="A29" t="s">
         <v>117</v>
       </c>
-      <c r="B29" s="17">
-        <v>1</v>
-      </c>
-      <c r="C29" s="18" t="s">
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
         <v>118</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" t="s">
         <v>119</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="17">
+      <c r="E29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" s="1">
         <v>22</v>
       </c>
       <c r="G29" s="1">
@@ -3163,22 +3382,22 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+      <c r="A30" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="17">
+      <c r="B30" s="1">
         <v>2</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" t="s">
         <v>121</v>
       </c>
-      <c r="E30" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" s="17">
+      <c r="E30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" s="1">
         <v>19</v>
       </c>
       <c r="G30" s="1">
@@ -3445,22 +3664,22 @@
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
+      <c r="A36" t="s">
         <v>57</v>
       </c>
-      <c r="B36" s="17">
-        <v>1</v>
-      </c>
-      <c r="C36" s="18" t="s">
+      <c r="B36" s="1">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" t="s">
         <v>84</v>
       </c>
-      <c r="E36" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F36" s="17">
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="1">
         <v>8</v>
       </c>
       <c r="G36" s="1">
@@ -3633,22 +3852,22 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="5">
+      <c r="B40" s="20">
         <v>2</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="D40" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="20">
         <v>28</v>
       </c>
       <c r="G40" s="1">
@@ -3680,22 +3899,22 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="20">
         <v>3</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="D41" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="5" t="s">
+      <c r="E41" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="20">
         <v>36</v>
       </c>
       <c r="G41" s="1">
@@ -3727,22 +3946,22 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A42" s="18" t="s">
+      <c r="A42" t="s">
         <v>131</v>
       </c>
-      <c r="B42" s="17">
-        <v>1</v>
-      </c>
-      <c r="C42" s="18" t="s">
+      <c r="B42" s="1">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
         <v>132</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" t="s">
         <v>133</v>
       </c>
-      <c r="E42" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="17">
+      <c r="E42" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" s="1">
         <v>34</v>
       </c>
       <c r="G42" s="1">
@@ -3774,22 +3993,22 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A43" s="18" t="s">
+      <c r="A43" t="s">
         <v>131</v>
       </c>
-      <c r="B43" s="17">
+      <c r="B43" s="1">
         <v>2</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" t="s">
         <v>135</v>
       </c>
-      <c r="E43" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="17">
+      <c r="E43" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="1">
         <v>15</v>
       </c>
       <c r="G43" s="1">
@@ -3821,22 +4040,22 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A44" s="18" t="s">
+      <c r="A44" t="s">
         <v>131</v>
       </c>
-      <c r="B44" s="17">
+      <c r="B44" s="1">
         <v>3</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" t="s">
         <v>136</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D44" t="s">
         <v>137</v>
       </c>
-      <c r="E44" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="17">
+      <c r="E44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" s="1">
         <v>12</v>
       </c>
       <c r="G44" s="1">
@@ -4150,22 +4369,22 @@
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+      <c r="A51" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="20">
         <v>4</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="C51" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="E51" s="5" t="s">
+      <c r="E51" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="5">
+      <c r="F51" s="20">
         <v>14</v>
       </c>
       <c r="G51" s="1">
@@ -4195,6 +4414,14 @@
       <c r="O51" s="1">
         <v>1</v>
       </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A52" s="19"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="19"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -4211,8 +4438,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D5ACC4-4F75-46C3-931B-94A525DB3F50}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4251,13 +4478,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="6">
         <f>SUM(F3:F5)</f>
         <v>106</v>
@@ -4333,13 +4560,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
       <c r="F6" s="6">
         <f>SUM(F7:F11)</f>
         <v>108</v>
@@ -4461,13 +4688,13 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="6">
         <f>SUM(F13:F19)</f>
         <v>153</v>
@@ -4635,13 +4862,13 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="17" t="s">
         <v>166</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="6">
         <f>SUM(F21:F25)</f>
         <v>104</v>
@@ -4720,22 +4947,22 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="17">
-        <v>1</v>
-      </c>
-      <c r="C24" s="18" t="s">
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F24" s="17">
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="1">
         <v>17</v>
       </c>
       <c r="G24">
@@ -4743,22 +4970,22 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="17">
+      <c r="B25" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" t="s">
         <v>44</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="17">
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1">
         <v>9</v>
       </c>
       <c r="G25">
@@ -4766,14 +4993,14 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
       <c r="H26" t="s">
         <v>172</v>
       </c>
@@ -4782,23 +5009,23 @@
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
       <c r="F28" s="6">
         <f>SUM(F29:F32)</f>
         <v>138</v>
@@ -4877,22 +5104,22 @@
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="20" t="s">
+      <c r="A32" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="17">
+      <c r="B32" s="1">
         <v>3</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" t="s">
         <v>46</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" t="s">
         <v>47</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="17">
+      <c r="E32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" s="1">
         <v>16</v>
       </c>
       <c r="G32">
@@ -4900,13 +5127,13 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="6">
         <f>SUM(F34:F40)</f>
         <v>169</v>
@@ -4985,22 +5212,22 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B37" s="17">
-        <v>1</v>
-      </c>
-      <c r="C37" s="18" t="s">
+      <c r="B37" s="1">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="17">
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="1">
         <v>8</v>
       </c>
       <c r="G37">
@@ -5008,22 +5235,22 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B38" s="17">
+      <c r="B38" s="1">
         <v>2</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="17">
+      <c r="E38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" s="1">
         <v>10</v>
       </c>
       <c r="G38">
@@ -5031,22 +5258,22 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="1">
         <v>3</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="17">
+      <c r="E39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="1">
         <v>10</v>
       </c>
       <c r="G39">

</xml_diff>

<commit_message>
Completed Week 1 of Fall 1
First module of Supervised ML, Unsupervised ML, Measurement Systems Analysis, and Modern Regression Analysis complete
</commit_message>
<xml_diff>
--- a/MSDS_Courses.xlsx
+++ b/MSDS_Courses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e79b3e2af0eb62e/Documents/GitHub/MSDS_Coursework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1785" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61239C8F-F6F7-4DBA-A4BF-0EBBCC93064F}"/>
+  <xr:revisionPtr revIDLastSave="1791" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F652A1FA-472E-457D-B502-6C4C4BDB29E2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -679,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -711,10 +711,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,6 +732,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1118,16 +1118,16 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="1">
         <v>28</v>
       </c>
       <c r="G3" s="1">
@@ -1162,16 +1162,16 @@
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="1">
         <v>36</v>
       </c>
       <c r="G4" s="1">
@@ -1341,46 +1341,46 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="20">
+      <c r="B8" s="1">
         <v>4</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" t="s">
         <v>159</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" t="s">
         <v>160</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="1">
         <v>14</v>
       </c>
-      <c r="G8" s="20">
-        <v>0</v>
-      </c>
-      <c r="H8" s="20">
-        <v>0</v>
-      </c>
-      <c r="I8" s="20">
-        <v>0</v>
-      </c>
-      <c r="J8" s="20">
-        <v>0</v>
-      </c>
-      <c r="K8" s="20">
-        <v>0</v>
-      </c>
-      <c r="L8" s="20">
-        <v>0</v>
-      </c>
-      <c r="M8" s="20">
-        <v>0</v>
-      </c>
-      <c r="N8" s="20">
-        <v>1</v>
-      </c>
-      <c r="O8" s="20">
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
         <v>1</v>
       </c>
     </row>
@@ -1665,94 +1665,94 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="20">
-        <v>1</v>
-      </c>
-      <c r="C15" s="19" t="s">
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="20">
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1">
         <v>17</v>
       </c>
-      <c r="G15" s="20">
-        <v>1</v>
-      </c>
-      <c r="H15" s="20">
-        <v>1</v>
-      </c>
-      <c r="I15" s="20">
-        <v>1</v>
-      </c>
-      <c r="J15" s="20">
-        <v>1</v>
-      </c>
-      <c r="K15" s="20">
-        <v>0</v>
-      </c>
-      <c r="L15" s="20">
-        <v>0</v>
-      </c>
-      <c r="M15" s="20">
-        <v>0</v>
-      </c>
-      <c r="N15" s="20">
-        <v>0</v>
-      </c>
-      <c r="O15" s="20">
+      <c r="G15" s="1">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <v>1</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="1">
+        <v>0</v>
+      </c>
+      <c r="O15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="20">
+      <c r="B16" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="20">
+      <c r="E16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="1">
         <v>9</v>
       </c>
-      <c r="G16" s="20">
-        <v>1</v>
-      </c>
-      <c r="H16" s="20">
-        <v>1</v>
-      </c>
-      <c r="I16" s="20">
-        <v>1</v>
-      </c>
-      <c r="J16" s="20">
-        <v>1</v>
-      </c>
-      <c r="K16" s="20">
-        <v>0</v>
-      </c>
-      <c r="L16" s="20">
-        <v>0</v>
-      </c>
-      <c r="M16" s="20">
-        <v>0</v>
-      </c>
-      <c r="N16" s="20">
-        <v>0</v>
-      </c>
-      <c r="O16" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <v>1</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B18" s="1">
         <v>2</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B19" s="1">
         <v>1</v>
       </c>
@@ -1886,9 +1886,8 @@
       <c r="O19" s="1">
         <v>0</v>
       </c>
-      <c r="P19" s="19"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B20" s="1">
         <v>2</v>
       </c>
@@ -1931,9 +1930,8 @@
       <c r="O20" s="1">
         <v>0</v>
       </c>
-      <c r="P20" s="19"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" s="1">
         <v>3</v>
       </c>
@@ -1976,7 +1974,6 @@
       <c r="O21" s="1">
         <v>0</v>
       </c>
-      <c r="P21" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O16" xr:uid="{6FDCB567-5E07-42C0-8D3A-079FDCB96AF6}">
@@ -1993,7 +1990,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O52"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2207,22 +2204,22 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="20">
-        <v>1</v>
-      </c>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="20">
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1">
         <v>17</v>
       </c>
       <c r="G5" s="1">
@@ -2254,22 +2251,22 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="1">
         <v>2</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="20">
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1">
         <v>9</v>
       </c>
       <c r="G6" s="1">
@@ -3852,22 +3849,22 @@
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A40" s="19" t="s">
+      <c r="A40" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="20">
+      <c r="B40" s="1">
         <v>2</v>
       </c>
-      <c r="C40" s="19" t="s">
+      <c r="C40" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" t="s">
         <v>36</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F40" s="20">
+      <c r="F40" s="1">
         <v>28</v>
       </c>
       <c r="G40" s="1">
@@ -3899,22 +3896,22 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A41" s="19" t="s">
+      <c r="A41" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="20">
+      <c r="B41" s="1">
         <v>3</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" t="s">
         <v>37</v>
       </c>
-      <c r="D41" s="19" t="s">
+      <c r="D41" t="s">
         <v>38</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F41" s="20">
+      <c r="F41" s="1">
         <v>36</v>
       </c>
       <c r="G41" s="1">
@@ -4369,22 +4366,22 @@
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A51" s="19" t="s">
+      <c r="A51" t="s">
         <v>152</v>
       </c>
-      <c r="B51" s="20">
+      <c r="B51" s="1">
         <v>4</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" t="s">
         <v>159</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="D51" t="s">
         <v>160</v>
       </c>
-      <c r="E51" s="20" t="s">
+      <c r="E51" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F51" s="20">
+      <c r="F51" s="1">
         <v>14</v>
       </c>
       <c r="G51" s="1">
@@ -4414,14 +4411,6 @@
       <c r="O51" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A52" s="19"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:O51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -4436,10 +4425,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D5ACC4-4F75-46C3-931B-94A525DB3F50}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4792,7 +4781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>105</v>
       </c>
@@ -4815,7 +4804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>105</v>
       </c>
@@ -4838,7 +4827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>105</v>
       </c>
@@ -4861,7 +4850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>166</v>
       </c>
@@ -4873,11 +4862,8 @@
         <f>SUM(F21:F25)</f>
         <v>104</v>
       </c>
-      <c r="H20">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>30</v>
       </c>
@@ -4900,7 +4886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>30</v>
       </c>
@@ -4923,7 +4909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>152</v>
       </c>
@@ -4946,7 +4932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>39</v>
       </c>
@@ -4969,7 +4955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>39</v>
       </c>
@@ -4992,7 +4978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
         <v>173</v>
       </c>
@@ -5004,11 +4990,8 @@
       <c r="H26" t="s">
         <v>172</v>
       </c>
-      <c r="M26">
-        <v>20.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>58</v>
       </c>
@@ -5018,7 +5001,7 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>168</v>
       </c>
@@ -5027,14 +5010,14 @@
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="6">
-        <f>SUM(F29:F32)</f>
-        <v>138</v>
+        <f>SUM(F29:F33)</f>
+        <v>146</v>
       </c>
       <c r="H28">
         <v>143</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>98</v>
       </c>
@@ -5057,7 +5040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>98</v>
       </c>
@@ -5080,7 +5063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="12" t="s">
         <v>138</v>
       </c>
@@ -5103,7 +5086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>39</v>
       </c>
@@ -5127,42 +5110,42 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" s="1">
+        <v>8</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="17"/>
-      <c r="F33" s="6">
-        <f>SUM(F34:F40)</f>
-        <v>169</v>
-      </c>
-      <c r="H33">
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="6">
+        <f>SUM(F35:F40)</f>
+        <v>161</v>
+      </c>
+      <c r="H34">
         <v>164</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B34" s="1">
-        <v>2</v>
-      </c>
-      <c r="C34" t="s">
-        <v>141</v>
-      </c>
-      <c r="D34" t="s">
-        <v>142</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="1">
-        <v>39</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -5170,65 +5153,65 @@
         <v>138</v>
       </c>
       <c r="B35" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F35" s="1">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="11" t="s">
-        <v>98</v>
+      <c r="A36" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="B36" s="1">
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F36" s="1">
+        <v>42</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" s="1">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="1">
         <v>60</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="1">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>71</v>
-      </c>
-      <c r="D37" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F37" s="1">
-        <v>8</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -5282,7 +5265,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A34:E34"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A12:E12"/>

</xml_diff>

<commit_message>
finished Week 2 of Fall 2
</commit_message>
<xml_diff>
--- a/MSDS_Courses.xlsx
+++ b/MSDS_Courses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e79b3e2af0eb62e/Documents/GitHub/MSDS_Coursework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1791" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F652A1FA-472E-457D-B502-6C4C4BDB29E2}"/>
+  <xr:revisionPtr revIDLastSave="1799" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C669448A-F9CA-409F-8496-1081C9E3ABF1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="174">
   <si>
     <t>Specialization</t>
   </si>
@@ -679,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -711,6 +711,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,10 +736,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1001,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDCB567-5E07-42C0-8D3A-079FDCB96AF6}">
-  <dimension ref="A1:P21"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1975,12 +1975,184 @@
         <v>0</v>
       </c>
     </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="20">
+        <v>3</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="20">
+        <v>16</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1</v>
+      </c>
+      <c r="O22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B23" s="20">
+        <v>1</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="20">
+        <v>39</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <v>1</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0</v>
+      </c>
+      <c r="N23" s="1">
+        <v>1</v>
+      </c>
+      <c r="O23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B24" s="20">
+        <v>2</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="20">
+        <v>38</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>1</v>
+      </c>
+      <c r="M24" s="1">
+        <v>0</v>
+      </c>
+      <c r="N24" s="1">
+        <v>1</v>
+      </c>
+      <c r="O24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B25" s="20">
+        <v>1</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="20">
+        <v>45</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1">
+        <v>0</v>
+      </c>
+      <c r="N25" s="1">
+        <v>0</v>
+      </c>
+      <c r="O25" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O16" xr:uid="{6FDCB567-5E07-42C0-8D3A-079FDCB96AF6}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O16">
-      <sortCondition ref="C1:C9"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:O16" xr:uid="{6FDCB567-5E07-42C0-8D3A-079FDCB96AF6}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O21">
     <sortCondition ref="C1:C21"/>
   </sortState>
@@ -1993,8 +2165,8 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2298,22 +2470,22 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="20">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="E7" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="20">
         <v>16</v>
       </c>
       <c r="G7" s="1">
@@ -3097,22 +3269,22 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B24" s="5">
-        <v>1</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="20">
+        <v>1</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E24" s="5" t="s">
+      <c r="E24" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="20">
         <v>39</v>
       </c>
       <c r="G24" s="1">
@@ -3144,22 +3316,22 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="20">
         <v>2</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="20">
         <v>38</v>
       </c>
       <c r="G25" s="1">
@@ -4084,22 +4256,22 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="A45" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="B45" s="5">
-        <v>1</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="B45" s="20">
+        <v>1</v>
+      </c>
+      <c r="C45" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F45" s="5">
+      <c r="F45" s="20">
         <v>45</v>
       </c>
       <c r="G45" s="1">
@@ -4427,8 +4599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D5ACC4-4F75-46C3-931B-94A525DB3F50}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Completed most work for Fall 1 classes. Note that Modern Regression Analysis course will be extended into Fall 2 minimester.
</commit_message>
<xml_diff>
--- a/MSDS_Courses.xlsx
+++ b/MSDS_Courses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e79b3e2af0eb62e/Documents/GitHub/MSDS_Coursework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1799" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C669448A-F9CA-409F-8496-1081C9E3ABF1}"/>
+  <xr:revisionPtr revIDLastSave="1868" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBACDAD2-7D06-4654-BDD3-83AAB8F92405}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Completed" sheetId="2" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Completed!$A$1:$O$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Not_Taken!$A$1:$O$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Not_Taken!$A$1:$O$42</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="179">
   <si>
     <t>Specialization</t>
   </si>
@@ -560,10 +560,25 @@
     <t>2025 Spring 1 (7 weeks)</t>
   </si>
   <si>
-    <t>* Apply for jobs</t>
-  </si>
-  <si>
     <t>Summer Break (3 weeks)</t>
+  </si>
+  <si>
+    <t>2026 Spring 1 (8 weeks)</t>
+  </si>
+  <si>
+    <t>Bayesian Statistics</t>
+  </si>
+  <si>
+    <t>DTSA 5726</t>
+  </si>
+  <si>
+    <t>Introduction to Bayesian Statistics for Data Science Applications</t>
+  </si>
+  <si>
+    <t>High Performance and Parallel Computing</t>
+  </si>
+  <si>
+    <t>2026 Spring 2 (7 weeks)</t>
   </si>
 </sst>
 </file>
@@ -656,13 +671,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -679,7 +694,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -711,10 +726,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,6 +747,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1001,10 +1016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDCB567-5E07-42C0-8D3A-079FDCB96AF6}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1976,19 +1991,19 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="20">
+      <c r="B22" s="1">
         <v>3</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" t="s">
         <v>47</v>
       </c>
-      <c r="E22" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F22" s="20">
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="1">
         <v>16</v>
       </c>
       <c r="G22" s="1">
@@ -2020,19 +2035,19 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B23" s="20">
-        <v>1</v>
-      </c>
-      <c r="C23" s="19" t="s">
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" t="s">
         <v>100</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="20">
+      <c r="F23" s="1">
         <v>39</v>
       </c>
       <c r="G23" s="1">
@@ -2064,19 +2079,19 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B24" s="20">
+      <c r="B24" s="1">
         <v>2</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" t="s">
         <v>102</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="20">
+      <c r="F24" s="1">
         <v>38</v>
       </c>
       <c r="G24" s="1">
@@ -2108,19 +2123,19 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="20">
-        <v>1</v>
-      </c>
-      <c r="C25" s="19" t="s">
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" t="s">
         <v>140</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="20">
+      <c r="F25" s="1">
         <v>45</v>
       </c>
       <c r="G25" s="1">
@@ -2149,6 +2164,147 @@
       </c>
       <c r="O25" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="5">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="5">
+        <v>60</v>
+      </c>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1">
+        <v>1</v>
+      </c>
+      <c r="M26" s="1">
+        <v>0</v>
+      </c>
+      <c r="N26" s="1">
+        <v>1</v>
+      </c>
+      <c r="O26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="5">
+        <v>39</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>1</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1">
+        <v>0</v>
+      </c>
+      <c r="N27" s="1">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="5">
+        <v>3</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="5">
+        <v>42</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0</v>
+      </c>
+      <c r="L28" s="1">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1">
+        <v>0</v>
+      </c>
+      <c r="N28" s="1">
+        <v>0</v>
+      </c>
+      <c r="O28" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2162,11 +2318,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2179,9 +2335,9 @@
     <col min="6" max="6" width="10.44140625" style="1" customWidth="1"/>
     <col min="7" max="8" width="9.33203125" style="1" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.21875" customWidth="1"/>
+    <col min="10" max="10" width="12.21875" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="14.77734375" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.109375" style="1" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="8.88671875" style="1"/>
     <col min="14" max="14" width="9.6640625" style="1" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="1" hidden="1" customWidth="1"/>
@@ -2377,22 +2533,22 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F5" s="1">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="G5" s="1">
         <v>1</v>
@@ -2404,43 +2560,43 @@
         <v>1</v>
       </c>
       <c r="J5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="1">
         <v>0</v>
       </c>
       <c r="N5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1">
         <v>44</v>
       </c>
-      <c r="D6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="1">
-        <v>9</v>
-      </c>
       <c r="G6" s="1">
         <v>1</v>
       </c>
@@ -2451,54 +2607,54 @@
         <v>1</v>
       </c>
       <c r="J6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" s="1">
         <v>0</v>
       </c>
       <c r="N6" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="20">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1">
         <v>3</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="20">
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1">
         <v>16</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="1">
         <v>0</v>
@@ -2518,87 +2674,87 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>163</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="1">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="G8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="1">
         <v>0</v>
       </c>
       <c r="N8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="B9" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="1">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
       </c>
       <c r="K9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="1">
         <v>0</v>
@@ -2607,27 +2763,27 @@
         <v>1</v>
       </c>
       <c r="O9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>162</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>165</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="1">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -2662,19 +2818,19 @@
         <v>59</v>
       </c>
       <c r="B11" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>163</v>
+        <v>62</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -2698,7 +2854,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" s="1">
         <v>1</v>
@@ -2706,22 +2862,22 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>164</v>
+        <v>65</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F12" s="1">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -2745,30 +2901,30 @@
         <v>0</v>
       </c>
       <c r="N12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>67</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F13" s="1">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -2792,24 +2948,24 @@
         <v>0</v>
       </c>
       <c r="N13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>7</v>
@@ -2842,33 +2998,33 @@
         <v>1</v>
       </c>
       <c r="O14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F15" s="1">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="1">
         <v>0</v>
@@ -2880,13 +3036,13 @@
         <v>0</v>
       </c>
       <c r="L15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M15" s="1">
         <v>0</v>
       </c>
       <c r="N15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="1">
         <v>0</v>
@@ -2894,28 +3050,28 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B16" s="1">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D16" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F16" s="1">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="1">
         <v>0</v>
@@ -2927,13 +3083,13 @@
         <v>0</v>
       </c>
       <c r="L16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="1">
         <v>0</v>
       </c>
       <c r="N16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="1">
         <v>0</v>
@@ -2941,28 +3097,28 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="B17" s="1">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F17" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="1">
         <v>0</v>
@@ -2974,7 +3130,7 @@
         <v>0</v>
       </c>
       <c r="L17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M17" s="1">
         <v>0</v>
@@ -2983,33 +3139,33 @@
         <v>1</v>
       </c>
       <c r="O17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="5">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="5">
-        <v>8</v>
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1">
+        <v>27</v>
       </c>
       <c r="G18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="1">
         <v>0</v>
@@ -3021,10 +3177,10 @@
         <v>0</v>
       </c>
       <c r="L18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="1">
         <v>1</v>
@@ -3034,29 +3190,29 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="5">
+      <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="1">
         <v>2</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="5">
-        <v>10</v>
+      <c r="C19" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="1">
+        <v>25</v>
       </c>
       <c r="G19" s="1">
         <v>1</v>
       </c>
       <c r="H19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1">
         <v>0</v>
@@ -3068,10 +3224,10 @@
         <v>0</v>
       </c>
       <c r="L19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="1">
         <v>1</v>
@@ -3081,29 +3237,29 @@
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="5">
+      <c r="A20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="1">
         <v>3</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="5">
-        <v>10</v>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" s="1">
+        <v>42</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
       </c>
       <c r="H20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="1">
         <v>0</v>
@@ -3115,86 +3271,86 @@
         <v>0</v>
       </c>
       <c r="L20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="1">
         <v>1</v>
       </c>
       <c r="O20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="1">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" t="s">
-        <v>93</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="1">
-        <v>27</v>
+      <c r="A21" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="5">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="5">
+        <v>60</v>
       </c>
       <c r="G21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="1">
         <v>0</v>
       </c>
       <c r="L21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N21" s="1">
         <v>1</v>
       </c>
       <c r="O21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="B22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F22" s="1">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
         <v>0</v>
@@ -3212,10 +3368,10 @@
         <v>0</v>
       </c>
       <c r="M22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O22" s="1">
         <v>0</v>
@@ -3223,25 +3379,25 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="B23" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F23" s="1">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="G23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="1">
         <v>0</v>
@@ -3259,33 +3415,33 @@
         <v>0</v>
       </c>
       <c r="M23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O23" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="20">
-        <v>1</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="20">
-        <v>39</v>
+      <c r="A24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>118</v>
+      </c>
+      <c r="D24" t="s">
+        <v>119</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="1">
+        <v>22</v>
       </c>
       <c r="G24" s="1">
         <v>1</v>
@@ -3297,10 +3453,10 @@
         <v>1</v>
       </c>
       <c r="J24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L24" s="1">
         <v>1</v>
@@ -3309,30 +3465,30 @@
         <v>0</v>
       </c>
       <c r="N24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O24" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="20">
+      <c r="A25" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="1">
         <v>2</v>
       </c>
-      <c r="C25" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="20">
-        <v>38</v>
+      <c r="C25" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" t="s">
+        <v>121</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" s="1">
+        <v>19</v>
       </c>
       <c r="G25" s="1">
         <v>1</v>
@@ -3344,10 +3500,10 @@
         <v>1</v>
       </c>
       <c r="J25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25" s="1">
         <v>1</v>
@@ -3356,77 +3512,77 @@
         <v>0</v>
       </c>
       <c r="N25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" s="5">
-        <v>3</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="5">
-        <v>60</v>
+      <c r="A26" t="s">
+        <v>124</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D26" t="s">
+        <v>126</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" s="1">
+        <v>23</v>
       </c>
       <c r="G26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K26" s="1">
         <v>0</v>
       </c>
       <c r="L26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="1">
         <v>0</v>
       </c>
       <c r="N26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="D27" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F27" s="1">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G27" s="1">
         <v>0</v>
@@ -3458,22 +3614,22 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B28" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="D28" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F28" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G28" s="1">
         <v>0</v>
@@ -3497,51 +3653,51 @@
         <v>0</v>
       </c>
       <c r="N28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>117</v>
+        <v>177</v>
       </c>
       <c r="B29" s="1">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>118</v>
+        <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>119</v>
+        <v>86</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F29" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="1">
         <v>0</v>
       </c>
       <c r="K29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="1">
         <v>0</v>
@@ -3552,43 +3708,43 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>117</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" t="s">
-        <v>120</v>
+        <v>87</v>
       </c>
       <c r="D30" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F30" s="1">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" s="1">
         <v>0</v>
       </c>
       <c r="K30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" s="1">
         <v>0</v>
@@ -3599,28 +3755,28 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>125</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F31" s="1">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="G31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="1">
         <v>0</v>
@@ -3632,13 +3788,13 @@
         <v>0</v>
       </c>
       <c r="L31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="1">
         <v>0</v>
       </c>
       <c r="N31" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O31" s="1">
         <v>0</v>
@@ -3646,22 +3802,22 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="B32" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F32" s="1">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="G32" s="1">
         <v>0</v>
@@ -3693,28 +3849,28 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>57</v>
       </c>
       <c r="B33" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="D33" t="s">
-        <v>130</v>
+        <v>55</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F33" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" s="1">
         <v>0</v>
@@ -3726,16 +3882,16 @@
         <v>0</v>
       </c>
       <c r="L33" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="1">
         <v>0</v>
       </c>
       <c r="N33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
@@ -3746,16 +3902,16 @@
         <v>1</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F34" s="1">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
@@ -3787,34 +3943,34 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B35" s="1">
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="D35" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F35" s="1">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="G35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="1">
         <v>0</v>
@@ -3823,33 +3979,33 @@
         <v>0</v>
       </c>
       <c r="M35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35" s="1">
         <v>0</v>
       </c>
       <c r="O35" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B36" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="D36" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F36" s="1">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G36" s="1">
         <v>1</v>
@@ -3858,57 +4014,57 @@
         <v>1</v>
       </c>
       <c r="I36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="1">
         <v>0</v>
       </c>
       <c r="L36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M36" s="1">
         <v>0</v>
       </c>
       <c r="N36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O36" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>131</v>
       </c>
       <c r="B37" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F37" s="1">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="G37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="1">
         <v>0</v>
@@ -3923,27 +4079,27 @@
         <v>0</v>
       </c>
       <c r="O37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="1">
-        <v>1</v>
-      </c>
-      <c r="C38" t="s">
-        <v>56</v>
-      </c>
-      <c r="D38" t="s">
-        <v>55</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F38" s="1">
-        <v>20</v>
+      <c r="A38" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="5">
+        <v>2</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="5">
+        <v>39</v>
       </c>
       <c r="G38" s="1">
         <v>1</v>
@@ -3952,10 +4108,10 @@
         <v>1</v>
       </c>
       <c r="I38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="1">
         <v>0</v>
@@ -3970,83 +4126,83 @@
         <v>0</v>
       </c>
       <c r="O38" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>57</v>
-      </c>
-      <c r="B39" s="1">
-        <v>1</v>
-      </c>
-      <c r="C39" t="s">
-        <v>122</v>
-      </c>
-      <c r="D39" t="s">
-        <v>123</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="1">
-        <v>18</v>
+      <c r="A39" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="5">
+        <v>3</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="5">
+        <v>42</v>
       </c>
       <c r="G39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="1">
         <v>0</v>
       </c>
       <c r="L39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N39" s="1">
         <v>0</v>
       </c>
       <c r="O39" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>145</v>
       </c>
       <c r="B40" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>146</v>
       </c>
       <c r="D40" t="s">
-        <v>36</v>
+        <v>147</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F40" s="1">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="G40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" s="1">
         <v>0</v>
@@ -4061,39 +4217,39 @@
         <v>0</v>
       </c>
       <c r="N40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O40" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>145</v>
       </c>
       <c r="B41" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>148</v>
       </c>
       <c r="D41" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F41" s="1">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="G41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" s="1">
         <v>0</v>
@@ -4108,42 +4264,42 @@
         <v>0</v>
       </c>
       <c r="N41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O41" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B42" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="D42" t="s">
-        <v>133</v>
+        <v>151</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F42" s="1">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="G42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K42" s="1">
         <v>0</v>
@@ -4163,432 +4319,29 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="B43" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" t="s">
-        <v>134</v>
+        <v>175</v>
       </c>
       <c r="D43" t="s">
-        <v>135</v>
+        <v>176</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F43" s="1">
-        <v>15</v>
-      </c>
-      <c r="G43" s="1">
-        <v>1</v>
-      </c>
-      <c r="H43" s="1">
-        <v>1</v>
-      </c>
-      <c r="I43" s="1">
-        <v>1</v>
-      </c>
-      <c r="J43" s="1">
-        <v>1</v>
-      </c>
-      <c r="K43" s="1">
-        <v>0</v>
-      </c>
-      <c r="L43" s="1">
-        <v>0</v>
-      </c>
-      <c r="M43" s="1">
-        <v>0</v>
-      </c>
-      <c r="N43" s="1">
-        <v>0</v>
-      </c>
-      <c r="O43" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>131</v>
-      </c>
-      <c r="B44" s="1">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="1">
-        <v>12</v>
-      </c>
-      <c r="G44" s="1">
-        <v>1</v>
-      </c>
-      <c r="H44" s="1">
-        <v>1</v>
-      </c>
-      <c r="I44" s="1">
-        <v>1</v>
-      </c>
-      <c r="J44" s="1">
-        <v>1</v>
-      </c>
-      <c r="K44" s="1">
-        <v>0</v>
-      </c>
-      <c r="L44" s="1">
-        <v>0</v>
-      </c>
-      <c r="M44" s="1">
-        <v>0</v>
-      </c>
-      <c r="N44" s="1">
-        <v>0</v>
-      </c>
-      <c r="O44" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A45" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="B45" s="20">
-        <v>1</v>
-      </c>
-      <c r="C45" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="20">
-        <v>45</v>
-      </c>
-      <c r="G45" s="1">
-        <v>1</v>
-      </c>
-      <c r="H45" s="1">
-        <v>1</v>
-      </c>
-      <c r="I45" s="1">
-        <v>1</v>
-      </c>
-      <c r="J45" s="1">
-        <v>0</v>
-      </c>
-      <c r="K45" s="1">
-        <v>0</v>
-      </c>
-      <c r="L45" s="1">
-        <v>1</v>
-      </c>
-      <c r="M45" s="1">
-        <v>0</v>
-      </c>
-      <c r="N45" s="1">
-        <v>0</v>
-      </c>
-      <c r="O45" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B46" s="5">
-        <v>2</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" s="5">
-        <v>39</v>
-      </c>
-      <c r="G46" s="1">
-        <v>1</v>
-      </c>
-      <c r="H46" s="1">
-        <v>1</v>
-      </c>
-      <c r="I46" s="1">
-        <v>1</v>
-      </c>
-      <c r="J46" s="1">
-        <v>1</v>
-      </c>
-      <c r="K46" s="1">
-        <v>0</v>
-      </c>
-      <c r="L46" s="1">
-        <v>1</v>
-      </c>
-      <c r="M46" s="1">
-        <v>0</v>
-      </c>
-      <c r="N46" s="1">
-        <v>0</v>
-      </c>
-      <c r="O46" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B47" s="5">
-        <v>3</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F47" s="5">
-        <v>42</v>
-      </c>
-      <c r="G47" s="1">
-        <v>1</v>
-      </c>
-      <c r="H47" s="1">
-        <v>1</v>
-      </c>
-      <c r="I47" s="1">
-        <v>1</v>
-      </c>
-      <c r="J47" s="1">
-        <v>1</v>
-      </c>
-      <c r="K47" s="1">
-        <v>0</v>
-      </c>
-      <c r="L47" s="1">
-        <v>1</v>
-      </c>
-      <c r="M47" s="1">
-        <v>0</v>
-      </c>
-      <c r="N47" s="1">
-        <v>0</v>
-      </c>
-      <c r="O47" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>145</v>
-      </c>
-      <c r="B48" s="1">
-        <v>1</v>
-      </c>
-      <c r="C48" t="s">
-        <v>146</v>
-      </c>
-      <c r="D48" t="s">
-        <v>147</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F48" s="1">
-        <v>12</v>
-      </c>
-      <c r="G48" s="1">
-        <v>0</v>
-      </c>
-      <c r="H48" s="1">
-        <v>0</v>
-      </c>
-      <c r="I48" s="1">
-        <v>0</v>
-      </c>
-      <c r="J48" s="1">
-        <v>0</v>
-      </c>
-      <c r="K48" s="1">
-        <v>0</v>
-      </c>
-      <c r="L48" s="1">
-        <v>0</v>
-      </c>
-      <c r="M48" s="1">
-        <v>0</v>
-      </c>
-      <c r="N48" s="1">
-        <v>0</v>
-      </c>
-      <c r="O48" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>145</v>
-      </c>
-      <c r="B49" s="1">
-        <v>2</v>
-      </c>
-      <c r="C49" t="s">
-        <v>148</v>
-      </c>
-      <c r="D49" t="s">
-        <v>149</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F49" s="1">
-        <v>13</v>
-      </c>
-      <c r="G49" s="1">
-        <v>0</v>
-      </c>
-      <c r="H49" s="1">
-        <v>0</v>
-      </c>
-      <c r="I49" s="1">
-        <v>0</v>
-      </c>
-      <c r="J49" s="1">
-        <v>0</v>
-      </c>
-      <c r="K49" s="1">
-        <v>0</v>
-      </c>
-      <c r="L49" s="1">
-        <v>0</v>
-      </c>
-      <c r="M49" s="1">
-        <v>0</v>
-      </c>
-      <c r="N49" s="1">
-        <v>0</v>
-      </c>
-      <c r="O49" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>145</v>
-      </c>
-      <c r="B50" s="1">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>150</v>
-      </c>
-      <c r="D50" t="s">
-        <v>151</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F50" s="1">
-        <v>10</v>
-      </c>
-      <c r="G50" s="1">
-        <v>0</v>
-      </c>
-      <c r="H50" s="1">
-        <v>0</v>
-      </c>
-      <c r="I50" s="1">
-        <v>0</v>
-      </c>
-      <c r="J50" s="1">
-        <v>0</v>
-      </c>
-      <c r="K50" s="1">
-        <v>0</v>
-      </c>
-      <c r="L50" s="1">
-        <v>0</v>
-      </c>
-      <c r="M50" s="1">
-        <v>0</v>
-      </c>
-      <c r="N50" s="1">
-        <v>0</v>
-      </c>
-      <c r="O50" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>152</v>
-      </c>
-      <c r="B51" s="1">
-        <v>4</v>
-      </c>
-      <c r="C51" t="s">
-        <v>159</v>
-      </c>
-      <c r="D51" t="s">
-        <v>160</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F51" s="1">
-        <v>14</v>
-      </c>
-      <c r="G51" s="1">
-        <v>0</v>
-      </c>
-      <c r="H51" s="1">
-        <v>0</v>
-      </c>
-      <c r="I51" s="1">
-        <v>0</v>
-      </c>
-      <c r="J51" s="1">
-        <v>0</v>
-      </c>
-      <c r="K51" s="1">
-        <v>0</v>
-      </c>
-      <c r="L51" s="1">
-        <v>0</v>
-      </c>
-      <c r="M51" s="1">
-        <v>0</v>
-      </c>
-      <c r="N51" s="1">
-        <v>1</v>
-      </c>
-      <c r="O51" s="1">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:M51">
-    <sortCondition ref="B2:B51"/>
-    <sortCondition ref="F2:F51"/>
+  <autoFilter ref="A1:O42" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:M42">
+    <sortCondition ref="B2:B42"/>
+    <sortCondition ref="F2:F42"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4597,10 +4350,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D5ACC4-4F75-46C3-931B-94A525DB3F50}">
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4634,7 +4387,7 @@
         <v>161</v>
       </c>
       <c r="G1">
-        <f>SUM(G2:G59)</f>
+        <f>SUM(G2:G52)</f>
         <v>30</v>
       </c>
     </row>
@@ -4953,7 +4706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>105</v>
       </c>
@@ -4976,7 +4729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>105</v>
       </c>
@@ -4999,7 +4752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>105</v>
       </c>
@@ -5022,7 +4775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
         <v>166</v>
       </c>
@@ -5035,7 +4788,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>30</v>
       </c>
@@ -5058,7 +4811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
         <v>30</v>
       </c>
@@ -5081,7 +4834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>152</v>
       </c>
@@ -5104,8 +4857,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="16" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="1">
@@ -5127,8 +4880,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="15" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="1">
@@ -5150,20 +4903,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="17" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
       <c r="E26" s="17"/>
       <c r="F26" s="17"/>
-      <c r="H26" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>58</v>
       </c>
@@ -5173,7 +4923,7 @@
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="17" t="s">
         <v>168</v>
       </c>
@@ -5182,14 +4932,11 @@
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="6">
-        <f>SUM(F29:F33)</f>
-        <v>146</v>
-      </c>
-      <c r="H28">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+        <f>SUM(F29:F31)</f>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>98</v>
       </c>
@@ -5212,7 +4959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>98</v>
       </c>
@@ -5235,209 +4982,234 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="1">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" s="1">
+        <v>16</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="6">
+        <f>SUM(F33:F35)</f>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B31" s="1">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
         <v>139</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
         <v>140</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F33" s="1">
         <v>45</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32" s="1">
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F34" s="1">
+        <v>11</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="1">
         <v>3</v>
       </c>
-      <c r="C32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="1">
-        <v>16</v>
-      </c>
-      <c r="G32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="1">
-        <v>1</v>
-      </c>
-      <c r="C33" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" t="s">
-        <v>72</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" s="1">
-        <v>8</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="6">
-        <f>SUM(F35:F40)</f>
-        <v>161</v>
-      </c>
-      <c r="H34">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="B35" s="1">
-        <v>2</v>
-      </c>
       <c r="C35" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="D35" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F35" s="1">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="12" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="6">
+        <f>SUM(F37:F38)</f>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B36" s="1">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>143</v>
-      </c>
-      <c r="D36" t="s">
-        <v>144</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="1">
-        <v>42</v>
-      </c>
-      <c r="G36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="11" t="s">
-        <v>98</v>
-      </c>
       <c r="B37" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>141</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
+        <v>142</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F37" s="1">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="15" t="s">
-        <v>70</v>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="B38" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="D38" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F38" s="1">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="1">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="6">
+        <f>SUM(F40:F41)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="B40" s="1">
         <v>3</v>
       </c>
-      <c r="C39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" t="s">
-        <v>76</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F39" s="1">
-        <v>10</v>
-      </c>
-      <c r="G39">
+      <c r="C40" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40" t="s">
+        <v>144</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="1">
+        <v>42</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41" s="1">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>175</v>
+      </c>
+      <c r="D41" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" s="1">
+        <v>38</v>
+      </c>
+      <c r="G41">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A34:E34"/>
+  <mergeCells count="10">
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A32:E32"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A6:E6"/>
     <mergeCell ref="A12:E12"/>

</xml_diff>

<commit_message>
Added SML coursework from online. Completed SML course.
</commit_message>
<xml_diff>
--- a/MSDS_Courses.xlsx
+++ b/MSDS_Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8e79b3e2af0eb62e/Documents/GitHub/MSDS_Coursework/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1868" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DBACDAD2-7D06-4654-BDD3-83AAB8F92405}"/>
+  <xr:revisionPtr revIDLastSave="1872" documentId="11_F25DC773A252ABDACC104846A95D540C5BDE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FCA0FD97-9F43-4DFC-B3A0-C97730D55ED3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4352,8 +4352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D5ACC4-4F75-46C3-931B-94A525DB3F50}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5015,7 +5015,7 @@
       <c r="E32" s="17"/>
       <c r="F32" s="6">
         <f>SUM(F33:F35)</f>
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -5065,23 +5065,23 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
-        <v>98</v>
+      <c r="A35" s="13" t="s">
+        <v>20</v>
       </c>
       <c r="B35" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F35" s="1">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -5097,7 +5097,7 @@
       <c r="E36" s="17"/>
       <c r="F36" s="6">
         <f>SUM(F37:F38)</f>
-        <v>87</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -5124,23 +5124,23 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
-        <v>20</v>
+      <c r="A38" s="11" t="s">
+        <v>98</v>
       </c>
       <c r="B38" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F38" s="1">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="G38">
         <v>1</v>

</xml_diff>